<commit_message>
updating the Readme file and doing some code cleaning
</commit_message>
<xml_diff>
--- a/CSV Files/Clusters Evaluation results/GOLD vs Clusters - SBERT.xlsx
+++ b/CSV Files/Clusters Evaluation results/GOLD vs Clusters - SBERT.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\USERS-Load\PycharmProjects\pythonProject\CVS Files\Ads prompt\01.08.22\annotation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\USERS-Load\PycharmProjects\pythonProject\CSV Files\Clusters Evaluation results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90A86C72-651B-41EC-AA08-D473BB9C27E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A0A7890-3467-480F-B50B-B10B72D35DD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -269,9 +269,6 @@
     <t>On the other side it could be an advantage for the children to wtach TV even at a so young age.</t>
   </si>
   <si>
-    <t>GOLD standards</t>
-  </si>
-  <si>
     <t>clusters \ Reference</t>
   </si>
   <si>
@@ -456,6 +453,9 @@
   </si>
   <si>
     <t>Auto calculated using manually assessted data for 5 items of each cluster</t>
+  </si>
+  <si>
+    <t>GOLDStandards</t>
   </si>
 </sst>
 </file>
@@ -865,7 +865,7 @@
   <dimension ref="A1:AA83"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -879,7 +879,7 @@
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>0</v>
@@ -888,67 +888,67 @@
         <v>1</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="G1" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" t="s">
         <v>81</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>82</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>83</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>84</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>85</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>86</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>87</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>88</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>89</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>90</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>91</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>92</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>93</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>94</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>95</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>96</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>97</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>98</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>99</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.3">
@@ -965,7 +965,7 @@
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -1039,7 +1039,7 @@
         <v>7</v>
       </c>
       <c r="G3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -1113,7 +1113,7 @@
         <v>3</v>
       </c>
       <c r="G4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -1187,7 +1187,7 @@
         <v>2</v>
       </c>
       <c r="G5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -1261,7 +1261,7 @@
         <v>16</v>
       </c>
       <c r="G6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -1335,7 +1335,7 @@
         <v>2</v>
       </c>
       <c r="G7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H7">
         <v>0</v>
@@ -1409,7 +1409,7 @@
         <v>16</v>
       </c>
       <c r="G8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H8">
         <v>0</v>
@@ -1483,7 +1483,7 @@
         <v>10</v>
       </c>
       <c r="G9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -1557,7 +1557,7 @@
         <v>16</v>
       </c>
       <c r="G10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H10">
         <v>0</v>
@@ -1631,7 +1631,7 @@
         <v>7</v>
       </c>
       <c r="G11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H11">
         <v>0</v>
@@ -1702,7 +1702,7 @@
         <v>10</v>
       </c>
       <c r="G12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H12">
         <v>0</v>
@@ -1776,7 +1776,7 @@
         <v>10</v>
       </c>
       <c r="G13" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H13">
         <v>0</v>
@@ -1850,7 +1850,7 @@
         <v>10</v>
       </c>
       <c r="G14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H14">
         <v>4</v>
@@ -1924,7 +1924,7 @@
         <v>16</v>
       </c>
       <c r="G15" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H15">
         <v>3</v>
@@ -1995,7 +1995,7 @@
         <v>16</v>
       </c>
       <c r="G16" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H16">
         <v>0</v>
@@ -2069,7 +2069,7 @@
         <v>6</v>
       </c>
       <c r="G17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H17">
         <v>0</v>
@@ -2143,7 +2143,7 @@
         <v>3</v>
       </c>
       <c r="G18" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H18" s="11">
         <v>5</v>
@@ -2217,7 +2217,7 @@
         <v>9</v>
       </c>
       <c r="G19" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H19">
         <v>0</v>
@@ -2291,7 +2291,7 @@
         <v>5</v>
       </c>
       <c r="G20" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H20">
         <v>0</v>
@@ -2365,7 +2365,7 @@
         <v>4</v>
       </c>
       <c r="G21" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H21" s="9">
         <v>13</v>
@@ -2423,7 +2423,7 @@
         <v>5</v>
       </c>
       <c r="AA21" s="9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="22" spans="1:27" x14ac:dyDescent="0.3">
@@ -2440,10 +2440,10 @@
         <v>16</v>
       </c>
       <c r="G22" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="H22" s="12" t="s">
         <v>122</v>
-      </c>
-      <c r="H22" s="12" t="s">
-        <v>123</v>
       </c>
       <c r="I22" s="12"/>
     </row>
@@ -2489,7 +2489,7 @@
         <v>16</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H25" s="2"/>
     </row>
@@ -2507,7 +2507,7 @@
         <v>16</v>
       </c>
       <c r="G26" s="13" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H26" s="13"/>
     </row>
@@ -2525,7 +2525,7 @@
         <v>16</v>
       </c>
       <c r="G27" s="13" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H27" s="13"/>
     </row>
@@ -2543,7 +2543,7 @@
         <v>13</v>
       </c>
       <c r="G28" s="13" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H28" s="13"/>
     </row>
@@ -2561,7 +2561,7 @@
         <v>13</v>
       </c>
       <c r="G29" s="13" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H29" s="13"/>
     </row>
@@ -2579,7 +2579,7 @@
         <v>13</v>
       </c>
       <c r="G30" s="13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H30" s="13"/>
     </row>
@@ -2597,7 +2597,7 @@
         <v>16</v>
       </c>
       <c r="G31" s="13" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H31" s="13"/>
     </row>
@@ -2615,7 +2615,7 @@
         <v>16</v>
       </c>
       <c r="G32" s="13" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H32" s="13"/>
     </row>
@@ -2647,7 +2647,7 @@
         <v>12</v>
       </c>
       <c r="G34" s="14" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H34" s="14"/>
     </row>
@@ -2707,7 +2707,7 @@
         <v>17</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
@@ -2724,7 +2724,7 @@
         <v>17</v>
       </c>
       <c r="G39" s="13" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -2741,7 +2741,7 @@
         <v>17</v>
       </c>
       <c r="G40" s="13" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
@@ -2758,7 +2758,7 @@
         <v>17</v>
       </c>
       <c r="G41" s="13" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.3">
@@ -2775,7 +2775,7 @@
         <v>10</v>
       </c>
       <c r="G42" s="13" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.3">
@@ -2792,7 +2792,7 @@
         <v>1</v>
       </c>
       <c r="G43" s="13" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
@@ -2809,7 +2809,7 @@
         <v>2</v>
       </c>
       <c r="G44" s="13" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.3">
@@ -2826,7 +2826,7 @@
         <v>1</v>
       </c>
       <c r="G45" s="13" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.3">
@@ -2843,7 +2843,7 @@
         <v>2</v>
       </c>
       <c r="G46" s="12" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
adding some test cases
</commit_message>
<xml_diff>
--- a/CSV Files/Clusters Evaluation results/GOLD vs Clusters - SBERT.xlsx
+++ b/CSV Files/Clusters Evaluation results/GOLD vs Clusters - SBERT.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\USERS-Load\PycharmProjects\pythonProject\CSV Files\Clusters Evaluation results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A0A7890-3467-480F-B50B-B10B72D35DD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1514B8AF-29E1-47A9-812F-C322052C89DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -864,8 +864,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA83"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R28" sqref="R28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -873,8 +873,8 @@
     <col min="2" max="2" width="141.6640625" customWidth="1"/>
     <col min="3" max="3" width="15.109375" style="2" customWidth="1"/>
     <col min="4" max="4" width="12.5546875" style="4" customWidth="1"/>
-    <col min="7" max="7" width="143.33203125" customWidth="1"/>
-    <col min="8" max="8" width="20.6640625" customWidth="1"/>
+    <col min="7" max="7" width="20.6640625" customWidth="1"/>
+    <col min="8" max="8" width="11.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.3">

</xml_diff>